<commit_message>
Reporte Distribucion: IdEstado y Distancia
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias Alfano\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Logictracker\Logictracker\Logictracker\src\Web\Logictracker\Logictracker.Web\ExcelTemplate\Logictracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,17 +15,18 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$S$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$T$11</definedName>
     <definedName name="Base">Informe!$C$7</definedName>
-    <definedName name="CONFIRMACION">Informe!$P$11</definedName>
+    <definedName name="CONFIRMACION">Informe!$Q$11</definedName>
     <definedName name="DATE">Informe!$E$11</definedName>
     <definedName name="DESCRIPCION">Informe!$I$11</definedName>
     <definedName name="Desde">Informe!$C$8</definedName>
+    <definedName name="DISTANCIA">Informe!$P$11</definedName>
     <definedName name="Distrito">Informe!$C$6</definedName>
     <definedName name="DURACION">Informe!$M$11</definedName>
     <definedName name="ENTRADA">Informe!$K$11</definedName>
     <definedName name="Hasta">Informe!$C$9</definedName>
-    <definedName name="HORARIO">Informe!$Q$11</definedName>
+    <definedName name="HORARIO">Informe!$R$11</definedName>
     <definedName name="KM">Informe!$N$11</definedName>
     <definedName name="MANUAL">Informe!$J$11</definedName>
     <definedName name="ORDEN">Informe!$F$11</definedName>
@@ -34,19 +35,19 @@
     <definedName name="PARENTI09">Informe!$D$11</definedName>
     <definedName name="PARENTI17">Informe!$B$11</definedName>
     <definedName name="PARENTI44">Informe!$H$11</definedName>
-    <definedName name="READ_INACTIVE">Informe!$S$11</definedName>
+    <definedName name="READ_INACTIVE">Informe!$T$11</definedName>
     <definedName name="RUTA">Informe!$A$11</definedName>
     <definedName name="SALIDA">Informe!$L$11</definedName>
     <definedName name="STATE">Informe!$O$11</definedName>
     <definedName name="Titulo">Informe!$C$1</definedName>
-    <definedName name="UNREAD_INACTIVE">Informe!$R$11</definedName>
+    <definedName name="UNREAD_INACTIVE">Informe!$S$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Funciones</t>
   </si>
@@ -118,6 +119,9 @@
   </si>
   <si>
     <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Distancia</t>
   </si>
 </sst>
 </file>
@@ -1112,10 +1116,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,14 +1135,14 @@
     <col min="10" max="12" width="12.140625" customWidth="1"/>
     <col min="13" max="13" width="13.140625" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17.85546875" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:20" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1147,59 +1151,59 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:19" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1209,7 +1213,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1256,19 +1260,22 @@
         <v>11</v>
       </c>
       <c r="P11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="10" t="s">
+      <c r="R11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="S11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="10" t="s">
+      <c r="T11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1285,12 +1292,13 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="9"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="4"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:S11"/>
+  <autoFilter ref="A11:T11"/>
   <pageMargins left="0.11811023622047244" right="0.11811023622047244" top="0.11811023622047244" bottom="0.11811023622047244" header="0" footer="0"/>
   <pageSetup scale="23" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
- BI Informe Viaje Recarga -LogsDatamart
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
@@ -15,39 +15,40 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$T$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$U$11</definedName>
     <definedName name="Base">Informe!$C$7</definedName>
-    <definedName name="CONFIRMACION">Informe!$Q$11</definedName>
+    <definedName name="CONFIRMACION">Informe!$R$11</definedName>
     <definedName name="DATE">Informe!$E$11</definedName>
     <definedName name="DESCRIPCION">Informe!$I$11</definedName>
     <definedName name="Desde">Informe!$C$8</definedName>
-    <definedName name="DISTANCIA">Informe!$P$11</definedName>
+    <definedName name="DIFERENCIA">Informe!$M$11</definedName>
+    <definedName name="DISTANCIA">Informe!$Q$11</definedName>
     <definedName name="Distrito">Informe!$C$6</definedName>
-    <definedName name="DURACION">Informe!$M$11</definedName>
-    <definedName name="ENTRADA">Informe!$K$11</definedName>
+    <definedName name="DURACION">Informe!$N$11</definedName>
+    <definedName name="ENTRADA">Informe!$J$11</definedName>
     <definedName name="Hasta">Informe!$C$9</definedName>
-    <definedName name="HORARIO">Informe!$R$11</definedName>
-    <definedName name="KM">Informe!$N$11</definedName>
-    <definedName name="MANUAL">Informe!$J$11</definedName>
+    <definedName name="HORARIO">Informe!$S$11</definedName>
+    <definedName name="KM">Informe!$O$11</definedName>
+    <definedName name="MANUAL">Informe!$L$11</definedName>
     <definedName name="ORDEN">Informe!$F$11</definedName>
     <definedName name="ORDEN_REAL">Informe!$G$11</definedName>
     <definedName name="PARENTI03">Informe!$C$11</definedName>
     <definedName name="PARENTI09">Informe!$D$11</definedName>
     <definedName name="PARENTI17">Informe!$B$11</definedName>
     <definedName name="PARENTI44">Informe!$H$11</definedName>
-    <definedName name="READ_INACTIVE">Informe!$T$11</definedName>
+    <definedName name="READ_INACTIVE">Informe!$U$11</definedName>
     <definedName name="RUTA">Informe!$A$11</definedName>
-    <definedName name="SALIDA">Informe!$L$11</definedName>
-    <definedName name="STATE">Informe!$O$11</definedName>
+    <definedName name="SALIDA">Informe!$K$11</definedName>
+    <definedName name="STATE">Informe!$P$11</definedName>
     <definedName name="Titulo">Informe!$C$1</definedName>
-    <definedName name="UNREAD_INACTIVE">Informe!$S$11</definedName>
+    <definedName name="UNREAD_INACTIVE">Informe!$T$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Funciones</t>
   </si>
@@ -122,6 +123,9 @@
   </si>
   <si>
     <t>Distancia</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1120,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,17 +1136,17 @@
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="10" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="16" width="16.42578125" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1151,59 +1155,59 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1213,7 +1217,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1242,40 +1246,43 @@
         <v>23</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="M11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="Q11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="R11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="S11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="T11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="10" t="s">
+      <c r="U11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1291,14 +1298,15 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="9"/>
+      <c r="P12" s="4"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="4"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:T11"/>
+  <autoFilter ref="A11:U11"/>
   <pageMargins left="0.11811023622047244" right="0.11811023622047244" top="0.11811023622047244" bottom="0.11811023622047244" header="0" footer="0"/>
   <pageSetup scale="23" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
PR 5: Merge dev to kafka_rq
 - Se agrega filtro fecha y columna usuario en documentos
 - Merge branch 'dev' of
 - cambios datamart y cambios en parser de cusat
 - MonitorCheckOut
 - Merge branch 'dev' of
 - ...
 - Correccion documentos filtro
 - Merge branch 'dev' of
 - Fix
 - Merge branch 'dev' of
...

Related work items: #258
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
@@ -15,39 +15,40 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$T$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$U$11</definedName>
     <definedName name="Base">Informe!$C$7</definedName>
-    <definedName name="CONFIRMACION">Informe!$Q$11</definedName>
+    <definedName name="CONFIRMACION">Informe!$R$11</definedName>
     <definedName name="DATE">Informe!$E$11</definedName>
     <definedName name="DESCRIPCION">Informe!$I$11</definedName>
     <definedName name="Desde">Informe!$C$8</definedName>
-    <definedName name="DISTANCIA">Informe!$P$11</definedName>
+    <definedName name="DIFERENCIA">Informe!$M$11</definedName>
+    <definedName name="DISTANCIA">Informe!$Q$11</definedName>
     <definedName name="Distrito">Informe!$C$6</definedName>
-    <definedName name="DURACION">Informe!$M$11</definedName>
-    <definedName name="ENTRADA">Informe!$K$11</definedName>
+    <definedName name="DURACION">Informe!$N$11</definedName>
+    <definedName name="ENTRADA">Informe!$J$11</definedName>
     <definedName name="Hasta">Informe!$C$9</definedName>
-    <definedName name="HORARIO">Informe!$R$11</definedName>
-    <definedName name="KM">Informe!$N$11</definedName>
-    <definedName name="MANUAL">Informe!$J$11</definedName>
+    <definedName name="HORARIO">Informe!$S$11</definedName>
+    <definedName name="KM">Informe!$O$11</definedName>
+    <definedName name="MANUAL">Informe!$L$11</definedName>
     <definedName name="ORDEN">Informe!$F$11</definedName>
     <definedName name="ORDEN_REAL">Informe!$G$11</definedName>
     <definedName name="PARENTI03">Informe!$C$11</definedName>
     <definedName name="PARENTI09">Informe!$D$11</definedName>
     <definedName name="PARENTI17">Informe!$B$11</definedName>
     <definedName name="PARENTI44">Informe!$H$11</definedName>
-    <definedName name="READ_INACTIVE">Informe!$T$11</definedName>
+    <definedName name="READ_INACTIVE">Informe!$U$11</definedName>
     <definedName name="RUTA">Informe!$A$11</definedName>
-    <definedName name="SALIDA">Informe!$L$11</definedName>
-    <definedName name="STATE">Informe!$O$11</definedName>
+    <definedName name="SALIDA">Informe!$K$11</definedName>
+    <definedName name="STATE">Informe!$P$11</definedName>
     <definedName name="Titulo">Informe!$C$1</definedName>
-    <definedName name="UNREAD_INACTIVE">Informe!$S$11</definedName>
+    <definedName name="UNREAD_INACTIVE">Informe!$T$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Funciones</t>
   </si>
@@ -122,6 +123,9 @@
   </si>
   <si>
     <t>Distancia</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1120,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,17 +1136,17 @@
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="10" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="16" width="16.42578125" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1151,59 +1155,59 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1213,7 +1217,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1242,40 +1246,43 @@
         <v>23</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="M11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="Q11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="R11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="S11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="T11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="10" t="s">
+      <c r="U11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1291,14 +1298,15 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="9"/>
+      <c r="P12" s="4"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="4"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:T11"/>
+  <autoFilter ref="A11:U11"/>
   <pageMargins left="0.11811023622047244" right="0.11811023622047244" top="0.11811023622047244" bottom="0.11811023622047244" header="0" footer="0"/>
   <pageSetup scale="23" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
PR 6: Merge dev to modulo_ordenes
 - geocoder en webapi
 - Filtro transportista
 - Revertir STrace y subir librerias dynamiproxy
 - Merge branch 'dev' of
 - cambios lojack web service
 - archivos faltantes lojack
 - Archivos faltantes modificacion lojack
 - referencia proyecto g4s
 - - BI Informe Viaje Recarga
 - Merge branch 'dev' of
...
</commit_message>
<xml_diff>
--- a/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
+++ b/Logictracker/Logictracker/src/Web/Logictracker/Logictracker.Web/ExcelTemplate/Logictracker/ReporteDistribucion.xlsx
@@ -15,39 +15,40 @@
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$T$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Informe!$A$11:$U$11</definedName>
     <definedName name="Base">Informe!$C$7</definedName>
-    <definedName name="CONFIRMACION">Informe!$Q$11</definedName>
+    <definedName name="CONFIRMACION">Informe!$R$11</definedName>
     <definedName name="DATE">Informe!$E$11</definedName>
     <definedName name="DESCRIPCION">Informe!$I$11</definedName>
     <definedName name="Desde">Informe!$C$8</definedName>
-    <definedName name="DISTANCIA">Informe!$P$11</definedName>
+    <definedName name="DIFERENCIA">Informe!$M$11</definedName>
+    <definedName name="DISTANCIA">Informe!$Q$11</definedName>
     <definedName name="Distrito">Informe!$C$6</definedName>
-    <definedName name="DURACION">Informe!$M$11</definedName>
-    <definedName name="ENTRADA">Informe!$K$11</definedName>
+    <definedName name="DURACION">Informe!$N$11</definedName>
+    <definedName name="ENTRADA">Informe!$J$11</definedName>
     <definedName name="Hasta">Informe!$C$9</definedName>
-    <definedName name="HORARIO">Informe!$R$11</definedName>
-    <definedName name="KM">Informe!$N$11</definedName>
-    <definedName name="MANUAL">Informe!$J$11</definedName>
+    <definedName name="HORARIO">Informe!$S$11</definedName>
+    <definedName name="KM">Informe!$O$11</definedName>
+    <definedName name="MANUAL">Informe!$L$11</definedName>
     <definedName name="ORDEN">Informe!$F$11</definedName>
     <definedName name="ORDEN_REAL">Informe!$G$11</definedName>
     <definedName name="PARENTI03">Informe!$C$11</definedName>
     <definedName name="PARENTI09">Informe!$D$11</definedName>
     <definedName name="PARENTI17">Informe!$B$11</definedName>
     <definedName name="PARENTI44">Informe!$H$11</definedName>
-    <definedName name="READ_INACTIVE">Informe!$T$11</definedName>
+    <definedName name="READ_INACTIVE">Informe!$U$11</definedName>
     <definedName name="RUTA">Informe!$A$11</definedName>
-    <definedName name="SALIDA">Informe!$L$11</definedName>
-    <definedName name="STATE">Informe!$O$11</definedName>
+    <definedName name="SALIDA">Informe!$K$11</definedName>
+    <definedName name="STATE">Informe!$P$11</definedName>
     <definedName name="Titulo">Informe!$C$1</definedName>
-    <definedName name="UNREAD_INACTIVE">Informe!$S$11</definedName>
+    <definedName name="UNREAD_INACTIVE">Informe!$T$11</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Funciones</t>
   </si>
@@ -122,6 +123,9 @@
   </si>
   <si>
     <t>Distancia</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1120,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,17 +1136,17 @@
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="10" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="16" width="16.42578125" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1151,59 +1155,59 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1213,7 +1217,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -1242,40 +1246,43 @@
         <v>23</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="M11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="Q11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="R11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="S11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="T11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="10" t="s">
+      <c r="U11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1291,14 +1298,15 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="9"/>
+      <c r="P12" s="4"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="4"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:T11"/>
+  <autoFilter ref="A11:U11"/>
   <pageMargins left="0.11811023622047244" right="0.11811023622047244" top="0.11811023622047244" bottom="0.11811023622047244" header="0" footer="0"/>
   <pageSetup scale="23" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>